<commit_message>
Added specific motor matrix
</commit_message>
<xml_diff>
--- a/Motor and Servo Decision Matrices.xlsx
+++ b/Motor and Servo Decision Matrices.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="65">
   <si>
     <t>motor</t>
   </si>
@@ -208,12 +208,18 @@
   </si>
   <si>
     <t>Cytron SPG30-60</t>
+  </si>
+  <si>
+    <t>Stall Current (A)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="1">
+    <numFmt numFmtId="172" formatCode="0.0"/>
+  </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -252,7 +258,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -261,11 +267,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="172" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -570,8 +578,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -579,8 +587,8 @@
     <col min="1" max="1" width="29.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="23.28515625" customWidth="1"/>
     <col min="3" max="3" width="17" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.28515625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="33.42578125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="16" customWidth="1"/>
   </cols>
@@ -607,7 +615,7 @@
       <c r="G1" t="s">
         <v>14</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="H1" s="6" t="s">
         <v>5</v>
       </c>
     </row>
@@ -633,7 +641,7 @@
       <c r="G2">
         <v>0.25</v>
       </c>
-      <c r="H2" s="4"/>
+      <c r="H2" s="6"/>
       <c r="I2" s="1"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
@@ -658,7 +666,7 @@
       <c r="G3" t="s">
         <v>17</v>
       </c>
-      <c r="J3" s="6" t="s">
+      <c r="J3" s="5" t="s">
         <v>22</v>
       </c>
     </row>
@@ -684,7 +692,7 @@
       <c r="G4" t="s">
         <v>12</v>
       </c>
-      <c r="J4" s="6" t="s">
+      <c r="J4" s="5" t="s">
         <v>30</v>
       </c>
     </row>
@@ -710,7 +718,7 @@
       <c r="G5" t="s">
         <v>17</v>
       </c>
-      <c r="J5" s="6" t="s">
+      <c r="J5" s="5" t="s">
         <v>26</v>
       </c>
     </row>
@@ -736,7 +744,7 @@
       <c r="G6" t="s">
         <v>18</v>
       </c>
-      <c r="J6" s="6" t="s">
+      <c r="J6" s="5" t="s">
         <v>27</v>
       </c>
     </row>
@@ -762,12 +770,12 @@
       <c r="G7" t="s">
         <v>13</v>
       </c>
-      <c r="J7" s="6" t="s">
+      <c r="J7" s="5" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="J8" s="6" t="s">
+      <c r="J8" s="5" t="s">
         <v>29</v>
       </c>
     </row>
@@ -793,7 +801,7 @@
       <c r="G9" t="s">
         <v>14</v>
       </c>
-      <c r="J9" s="6" t="s">
+      <c r="J9" s="5" t="s">
         <v>34</v>
       </c>
     </row>
@@ -966,15 +974,15 @@
         <v>20</v>
       </c>
       <c r="C17" t="s">
-        <v>21</v>
-      </c>
-      <c r="D17" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="D17" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="E17" s="5" t="s">
+      <c r="E17" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="F17" s="5" t="s">
+      <c r="F17" s="4" t="s">
         <v>59</v>
       </c>
       <c r="G17" t="s">
@@ -992,16 +1000,16 @@
       <c r="C18">
         <v>0.2</v>
       </c>
-      <c r="D18" s="5">
+      <c r="D18" s="4">
         <v>0.1</v>
       </c>
-      <c r="E18" s="5">
+      <c r="E18" s="4">
         <v>0.15</v>
       </c>
-      <c r="F18" s="5">
+      <c r="F18" s="4">
         <v>0.1</v>
       </c>
-      <c r="G18" s="5">
+      <c r="G18" s="4">
         <v>0.4</v>
       </c>
       <c r="H18" s="3"/>
@@ -1014,7 +1022,7 @@
         <v>1216</v>
       </c>
       <c r="C19">
-        <v>5000</v>
+        <v>5</v>
       </c>
       <c r="D19">
         <v>1.46</v>
@@ -1028,7 +1036,7 @@
       <c r="G19">
         <v>39.950000000000003</v>
       </c>
-      <c r="I19" s="6" t="s">
+      <c r="I19" s="5" t="s">
         <v>26</v>
       </c>
     </row>
@@ -1040,7 +1048,7 @@
         <v>180</v>
       </c>
       <c r="C20">
-        <v>1800</v>
+        <v>1.8</v>
       </c>
       <c r="D20">
         <v>1.46</v>
@@ -1054,7 +1062,7 @@
       <c r="G20">
         <v>22.58</v>
       </c>
-      <c r="I20" s="6" t="s">
+      <c r="I20" s="5" t="s">
         <v>27</v>
       </c>
     </row>
@@ -1066,7 +1074,7 @@
         <v>3200</v>
       </c>
       <c r="C21">
-        <v>5000</v>
+        <v>5</v>
       </c>
       <c r="D21">
         <v>1.46</v>
@@ -1080,7 +1088,7 @@
       <c r="G21">
         <v>39.950000000000003</v>
       </c>
-      <c r="I21" s="6" t="s">
+      <c r="I21" s="5" t="s">
         <v>28</v>
       </c>
     </row>
@@ -1092,7 +1100,7 @@
         <v>1920</v>
       </c>
       <c r="C22">
-        <v>3500</v>
+        <v>3.5</v>
       </c>
       <c r="D22">
         <v>0.48</v>
@@ -1106,7 +1114,7 @@
       <c r="G22">
         <v>24.99</v>
       </c>
-      <c r="I22" s="6" t="s">
+      <c r="I22" s="5" t="s">
         <v>58</v>
       </c>
     </row>
@@ -1120,13 +1128,13 @@
       <c r="C24" t="s">
         <v>21</v>
       </c>
-      <c r="D24" s="5" t="s">
+      <c r="D24" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="E24" s="5" t="s">
+      <c r="E24" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="F24" s="5" t="s">
+      <c r="F24" s="4" t="s">
         <v>59</v>
       </c>
       <c r="G24" t="s">
@@ -1146,16 +1154,16 @@
       <c r="C25">
         <v>0.2</v>
       </c>
-      <c r="D25" s="5">
+      <c r="D25" s="4">
         <v>0.1</v>
       </c>
-      <c r="E25" s="5">
+      <c r="E25" s="4">
         <v>0.15</v>
       </c>
-      <c r="F25" s="5">
+      <c r="F25" s="4">
         <v>0.1</v>
       </c>
-      <c r="G25" s="5">
+      <c r="G25" s="4">
         <v>0.4</v>
       </c>
       <c r="H25" s="3"/>
@@ -1168,30 +1176,30 @@
         <f>B19/$B$21*10</f>
         <v>3.8</v>
       </c>
-      <c r="C26">
+      <c r="C26" s="7">
         <f>C$20/C19*10</f>
         <v>3.5999999999999996</v>
       </c>
-      <c r="D26">
+      <c r="D26" s="7">
         <f>D$22/D19*10</f>
         <v>3.2876712328767121</v>
       </c>
-      <c r="E26">
+      <c r="E26" s="7">
         <f>E$20/E19*10</f>
         <v>8.8888888888888893</v>
       </c>
       <c r="F26">
         <v>5</v>
       </c>
-      <c r="G26">
+      <c r="G26" s="7">
         <f>G$20/G19*10</f>
         <v>5.6520650813516893</v>
       </c>
-      <c r="H26">
+      <c r="H26" s="7">
         <f>SUM(B26*B$25,C26*C$25,D26*D$25,E26*E$25,G26*G$25,F26*F$25)</f>
         <v>5.3329264891616805</v>
       </c>
-      <c r="I26" s="6" t="s">
+      <c r="I26" s="5" t="s">
         <v>26</v>
       </c>
     </row>
@@ -1199,7 +1207,7 @@
       <c r="A27" t="s">
         <v>63</v>
       </c>
-      <c r="B27">
+      <c r="B27" s="7">
         <f t="shared" ref="B27:B29" si="1">B20/$B$21*10</f>
         <v>0.5625</v>
       </c>
@@ -1207,26 +1215,26 @@
         <f t="shared" ref="C27:C29" si="2">C$20/C20*10</f>
         <v>10</v>
       </c>
-      <c r="D27">
+      <c r="D27" s="7">
         <f t="shared" ref="D27:D29" si="3">D$22/D20*10</f>
         <v>3.2876712328767121</v>
       </c>
-      <c r="E27">
+      <c r="E27" s="1">
         <f t="shared" ref="E27:E29" si="4">E$20/E20*10</f>
         <v>10</v>
       </c>
       <c r="F27">
         <v>10</v>
       </c>
-      <c r="G27">
+      <c r="G27" s="8">
         <f t="shared" ref="G27:G29" si="5">G$20/G20*10</f>
         <v>10</v>
       </c>
-      <c r="H27">
+      <c r="H27" s="7">
         <f>SUM(B27*B$25,C27*C$25,D27*D$25,E27*E$25,G27*G$25,F27*F$25)</f>
         <v>8.8568921232876718</v>
       </c>
-      <c r="I27" s="6" t="s">
+      <c r="I27" s="5" t="s">
         <v>27</v>
       </c>
     </row>
@@ -1242,26 +1250,26 @@
         <f t="shared" si="2"/>
         <v>3.5999999999999996</v>
       </c>
-      <c r="D28">
+      <c r="D28" s="7">
         <f t="shared" si="3"/>
         <v>3.2876712328767121</v>
       </c>
-      <c r="E28">
+      <c r="E28" s="7">
         <f t="shared" si="4"/>
         <v>8.8888888888888893</v>
       </c>
       <c r="F28">
         <v>5</v>
       </c>
-      <c r="G28">
+      <c r="G28" s="7">
         <f t="shared" si="5"/>
         <v>5.6520650813516893</v>
       </c>
-      <c r="H28">
+      <c r="H28" s="7">
         <f>SUM(B28*B$25,C28*C$25,D28*D$25,E28*E$25,G28*G$25,F28*F$25)</f>
         <v>5.6429264891616802</v>
       </c>
-      <c r="I28" s="6" t="s">
+      <c r="I28" s="5" t="s">
         <v>28</v>
       </c>
     </row>
@@ -1273,30 +1281,30 @@
         <f t="shared" si="1"/>
         <v>6</v>
       </c>
-      <c r="C29">
+      <c r="C29" s="7">
         <f t="shared" si="2"/>
-        <v>5.1428571428571423</v>
-      </c>
-      <c r="D29">
+        <v>5.1428571428571432</v>
+      </c>
+      <c r="D29" s="8">
         <f t="shared" si="3"/>
         <v>10</v>
       </c>
-      <c r="E29">
+      <c r="E29" s="7">
         <f t="shared" si="4"/>
         <v>5.1851851851851851</v>
       </c>
       <c r="F29">
         <v>0</v>
       </c>
-      <c r="G29">
+      <c r="G29" s="8">
         <f t="shared" si="5"/>
         <v>9.0356142456982784</v>
       </c>
-      <c r="H29">
+      <c r="H29" s="7">
         <f>SUM(B29*B$25,C29*C$25,D29*D$25,E29*E$25,G29*G$25,F29*F$25)</f>
         <v>6.7205949046285181</v>
       </c>
-      <c r="I29" s="6" t="s">
+      <c r="I29" s="5" t="s">
         <v>58</v>
       </c>
     </row>
@@ -1356,7 +1364,7 @@
       <c r="E1" t="s">
         <v>40</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="F1" s="6" t="s">
         <v>36</v>
       </c>
     </row>
@@ -1376,7 +1384,7 @@
       <c r="E2">
         <v>0.3</v>
       </c>
-      <c r="F2" s="4"/>
+      <c r="F2" s="6"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
@@ -1535,7 +1543,7 @@
       <c r="E11" t="s">
         <v>40</v>
       </c>
-      <c r="F11" s="4" t="s">
+      <c r="F11" s="6" t="s">
         <v>36</v>
       </c>
     </row>
@@ -1555,7 +1563,7 @@
       <c r="E12">
         <v>0.3</v>
       </c>
-      <c r="F12" s="4"/>
+      <c r="F12" s="6"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
@@ -1688,7 +1696,7 @@
         <f t="shared" si="3"/>
         <v>7.3434032509463378</v>
       </c>
-      <c r="G17" s="6" t="s">
+      <c r="G17" s="5" t="s">
         <v>51</v>
       </c>
     </row>

</xml_diff>

<commit_message>
started servos, and small fixes to motors
</commit_message>
<xml_diff>
--- a/Motor and Servo Decision Matrices.xlsx
+++ b/Motor and Servo Decision Matrices.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="135" windowWidth="18195" windowHeight="8505"/>
+    <workbookView xWindow="480" yWindow="135" windowWidth="18195" windowHeight="8505" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="motors" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="66">
   <si>
     <t>motor</t>
   </si>
@@ -211,6 +211,9 @@
   </si>
   <si>
     <t>Stall Current (A)</t>
+  </si>
+  <si>
+    <t>Precision</t>
   </si>
 </sst>
 </file>
@@ -218,7 +221,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="172" formatCode="0.0"/>
+    <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -269,11 +272,11 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="172" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -578,7 +581,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+    <sheetView topLeftCell="A6" workbookViewId="0">
       <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
@@ -615,7 +618,7 @@
       <c r="G1" t="s">
         <v>14</v>
       </c>
-      <c r="H1" s="6" t="s">
+      <c r="H1" s="8" t="s">
         <v>5</v>
       </c>
     </row>
@@ -641,7 +644,7 @@
       <c r="G2">
         <v>0.25</v>
       </c>
-      <c r="H2" s="6"/>
+      <c r="H2" s="8"/>
       <c r="I2" s="1"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
@@ -1176,26 +1179,26 @@
         <f>B19/$B$21*10</f>
         <v>3.8</v>
       </c>
-      <c r="C26" s="7">
+      <c r="C26" s="6">
         <f>C$20/C19*10</f>
         <v>3.5999999999999996</v>
       </c>
-      <c r="D26" s="7">
+      <c r="D26" s="6">
         <f>D$22/D19*10</f>
         <v>3.2876712328767121</v>
       </c>
-      <c r="E26" s="7">
+      <c r="E26" s="6">
         <f>E$20/E19*10</f>
         <v>8.8888888888888893</v>
       </c>
       <c r="F26">
         <v>5</v>
       </c>
-      <c r="G26" s="7">
+      <c r="G26" s="6">
         <f>G$20/G19*10</f>
         <v>5.6520650813516893</v>
       </c>
-      <c r="H26" s="7">
+      <c r="H26" s="6">
         <f>SUM(B26*B$25,C26*C$25,D26*D$25,E26*E$25,G26*G$25,F26*F$25)</f>
         <v>5.3329264891616805</v>
       </c>
@@ -1207,7 +1210,7 @@
       <c r="A27" t="s">
         <v>63</v>
       </c>
-      <c r="B27" s="7">
+      <c r="B27" s="6">
         <f t="shared" ref="B27:B29" si="1">B20/$B$21*10</f>
         <v>0.5625</v>
       </c>
@@ -1215,7 +1218,7 @@
         <f t="shared" ref="C27:C29" si="2">C$20/C20*10</f>
         <v>10</v>
       </c>
-      <c r="D27" s="7">
+      <c r="D27" s="6">
         <f t="shared" ref="D27:D29" si="3">D$22/D20*10</f>
         <v>3.2876712328767121</v>
       </c>
@@ -1226,11 +1229,11 @@
       <c r="F27">
         <v>10</v>
       </c>
-      <c r="G27" s="8">
+      <c r="G27" s="7">
         <f t="shared" ref="G27:G29" si="5">G$20/G20*10</f>
         <v>10</v>
       </c>
-      <c r="H27" s="7">
+      <c r="H27" s="6">
         <f>SUM(B27*B$25,C27*C$25,D27*D$25,E27*E$25,G27*G$25,F27*F$25)</f>
         <v>8.8568921232876718</v>
       </c>
@@ -1250,22 +1253,22 @@
         <f t="shared" si="2"/>
         <v>3.5999999999999996</v>
       </c>
-      <c r="D28" s="7">
+      <c r="D28" s="6">
         <f t="shared" si="3"/>
         <v>3.2876712328767121</v>
       </c>
-      <c r="E28" s="7">
+      <c r="E28" s="6">
         <f t="shared" si="4"/>
         <v>8.8888888888888893</v>
       </c>
       <c r="F28">
         <v>5</v>
       </c>
-      <c r="G28" s="7">
+      <c r="G28" s="6">
         <f t="shared" si="5"/>
         <v>5.6520650813516893</v>
       </c>
-      <c r="H28" s="7">
+      <c r="H28" s="6">
         <f>SUM(B28*B$25,C28*C$25,D28*D$25,E28*E$25,G28*G$25,F28*F$25)</f>
         <v>5.6429264891616802</v>
       </c>
@@ -1281,26 +1284,26 @@
         <f t="shared" si="1"/>
         <v>6</v>
       </c>
-      <c r="C29" s="7">
+      <c r="C29" s="6">
         <f t="shared" si="2"/>
         <v>5.1428571428571432</v>
       </c>
-      <c r="D29" s="8">
+      <c r="D29" s="7">
         <f t="shared" si="3"/>
         <v>10</v>
       </c>
-      <c r="E29" s="7">
+      <c r="E29" s="6">
         <f t="shared" si="4"/>
         <v>5.1851851851851851</v>
       </c>
       <c r="F29">
         <v>0</v>
       </c>
-      <c r="G29" s="8">
+      <c r="G29" s="7">
         <f t="shared" si="5"/>
         <v>9.0356142456982784</v>
       </c>
-      <c r="H29" s="7">
+      <c r="H29" s="6">
         <f>SUM(B29*B$25,C29*C$25,D29*D$25,E29*E$25,G29*G$25,F29*F$25)</f>
         <v>6.7205949046285181</v>
       </c>
@@ -1335,20 +1338,21 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G19"/>
+  <dimension ref="A1:H19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="44.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.5703125" customWidth="1"/>
+    <col min="4" max="5" width="17.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>35</v>
       </c>
@@ -1356,19 +1360,22 @@
         <v>43</v>
       </c>
       <c r="C1" t="s">
+        <v>65</v>
+      </c>
+      <c r="D1" t="s">
         <v>37</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>41</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>40</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="G1" s="8" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -1376,17 +1383,20 @@
         <v>0.2</v>
       </c>
       <c r="C2">
+        <v>0.3</v>
+      </c>
+      <c r="D2">
+        <v>0.1</v>
+      </c>
+      <c r="E2">
         <v>0.2</v>
       </c>
-      <c r="D2">
-        <v>0.3</v>
-      </c>
-      <c r="E2">
-        <v>0.3</v>
-      </c>
-      <c r="F2" s="6"/>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F2">
+        <v>0.2</v>
+      </c>
+      <c r="G2" s="8"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>38</v>
       </c>
@@ -1394,20 +1404,23 @@
         <v>2.38</v>
       </c>
       <c r="C3" t="s">
+        <v>61</v>
+      </c>
+      <c r="D3" t="s">
         <v>39</v>
       </c>
-      <c r="D3">
+      <c r="E3">
         <f>2.2*0.8*1.6</f>
         <v>2.8160000000000007</v>
       </c>
-      <c r="E3">
+      <c r="F3">
         <v>14</v>
       </c>
-      <c r="G3" t="s">
+      <c r="H3" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>42</v>
       </c>
@@ -1415,20 +1428,23 @@
         <v>1.39</v>
       </c>
       <c r="C4" t="s">
+        <v>60</v>
+      </c>
+      <c r="D4" t="s">
         <v>44</v>
       </c>
-      <c r="D4">
+      <c r="E4">
         <f>0.906*0.433*1.142</f>
         <v>0.44800431600000001</v>
       </c>
-      <c r="E4">
+      <c r="F4">
         <v>5.95</v>
       </c>
-      <c r="G4" t="s">
+      <c r="H4" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>45</v>
       </c>
@@ -1436,20 +1452,23 @@
         <v>5.625</v>
       </c>
       <c r="C5" t="s">
+        <v>60</v>
+      </c>
+      <c r="D5" t="s">
         <v>44</v>
       </c>
-      <c r="D5">
+      <c r="E5">
         <f>1.6*0.79*1.5</f>
         <v>1.8960000000000004</v>
       </c>
-      <c r="E5">
+      <c r="F5">
         <v>12</v>
       </c>
-      <c r="G5" t="s">
+      <c r="H5" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>49</v>
       </c>
@@ -1457,20 +1476,23 @@
         <v>1.18</v>
       </c>
       <c r="C6" t="s">
+        <v>60</v>
+      </c>
+      <c r="D6" t="s">
         <v>44</v>
       </c>
-      <c r="D6">
+      <c r="E6">
         <f>0.913*0.492*0.866</f>
         <v>0.38900373599999999</v>
       </c>
-      <c r="E6">
+      <c r="F6">
         <v>3.99</v>
       </c>
-      <c r="G6" t="s">
+      <c r="H6" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>50</v>
       </c>
@@ -1478,20 +1500,23 @@
         <v>1.18</v>
       </c>
       <c r="C7" t="s">
+        <v>61</v>
+      </c>
+      <c r="D7" t="s">
         <v>39</v>
       </c>
-      <c r="D7">
+      <c r="E7">
         <f>0.913*0.492*0.866</f>
         <v>0.38900373599999999</v>
       </c>
-      <c r="E7">
+      <c r="F7">
         <v>4.99</v>
       </c>
-      <c r="G7" t="s">
+      <c r="H7" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>53</v>
       </c>
@@ -1499,35 +1524,44 @@
         <v>1.3</v>
       </c>
       <c r="C8" t="s">
+        <v>60</v>
+      </c>
+      <c r="D8" t="s">
         <v>44</v>
       </c>
-      <c r="D8">
+      <c r="E8">
         <f>1.142*0.472*1.299</f>
         <v>0.70019217599999994</v>
       </c>
-      <c r="E8">
+      <c r="F8">
         <v>4.95</v>
       </c>
-      <c r="G8" t="s">
+      <c r="H8" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>56</v>
+      </c>
       <c r="B9">
         <v>2.169</v>
       </c>
       <c r="C9" t="s">
+        <v>60</v>
+      </c>
+      <c r="D9" t="s">
         <v>44</v>
       </c>
-      <c r="D9">
+      <c r="E9">
         <f>1.299*1.26*0.472</f>
         <v>0.77254127999999989</v>
       </c>
-      <c r="E9">
+      <c r="F9">
         <v>3.2</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>35</v>
       </c>
@@ -1535,37 +1569,43 @@
         <v>43</v>
       </c>
       <c r="C11" t="s">
+        <v>65</v>
+      </c>
+      <c r="D11" t="s">
         <v>37</v>
       </c>
-      <c r="D11" t="s">
+      <c r="E11" t="s">
         <v>41</v>
       </c>
-      <c r="E11" t="s">
+      <c r="F11" t="s">
         <v>40</v>
       </c>
-      <c r="F11" s="6" t="s">
+      <c r="G11" s="8" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>1</v>
       </c>
       <c r="B12" s="1">
         <v>0.2</v>
       </c>
-      <c r="C12">
+      <c r="C12" s="1">
+        <v>0.3</v>
+      </c>
+      <c r="D12">
+        <v>0.1</v>
+      </c>
+      <c r="E12">
         <v>0.2</v>
       </c>
-      <c r="D12">
-        <v>0.3</v>
-      </c>
-      <c r="E12">
-        <v>0.3</v>
-      </c>
-      <c r="F12" s="6"/>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F12">
+        <v>0.2</v>
+      </c>
+      <c r="G12" s="8"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>38</v>
       </c>
@@ -1573,26 +1613,29 @@
         <f>B3/B$5*10</f>
         <v>4.2311111111111108</v>
       </c>
-      <c r="C13">
-        <v>10</v>
-      </c>
-      <c r="D13" s="1">
-        <f>D$6/D3*10</f>
+      <c r="C13" s="1">
+        <v>5</v>
+      </c>
+      <c r="D13">
+        <v>10</v>
+      </c>
+      <c r="E13" s="1">
+        <f>E$6/E3*10</f>
         <v>1.3814053124999994</v>
       </c>
-      <c r="E13" s="1">
-        <f>E$9/E3*10</f>
+      <c r="F13" s="1">
+        <f>F$9/F3*10</f>
         <v>2.285714285714286</v>
       </c>
-      <c r="F13" s="1">
-        <f>SUM(B13*B$12,C13*C$12,D13*D$12,E13*E$12)</f>
-        <v>3.9463581016865077</v>
-      </c>
-      <c r="G13" t="s">
+      <c r="G13" s="1">
+        <f>SUM(B13*B$12,D13*D$12,E13*E$12,F13*F$12,C13*C$12)</f>
+        <v>4.07964614186508</v>
+      </c>
+      <c r="H13" s="5" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>42</v>
       </c>
@@ -1600,26 +1643,29 @@
         <f t="shared" ref="B14:B19" si="0">B4/B$5*10</f>
         <v>2.471111111111111</v>
       </c>
-      <c r="C14">
+      <c r="C14" s="1">
+        <v>10</v>
+      </c>
+      <c r="D14">
         <v>5</v>
       </c>
-      <c r="D14" s="1">
-        <f t="shared" ref="D14:D19" si="1">D$6/D4*10</f>
+      <c r="E14" s="1">
+        <f t="shared" ref="E14:E19" si="1">E$6/E4*10</f>
         <v>8.6830354553994962</v>
       </c>
-      <c r="E14" s="1">
-        <f t="shared" ref="E14:E19" si="2">E$9/E4*10</f>
+      <c r="F14" s="1">
+        <f t="shared" ref="F14:F19" si="2">F$9/F4*10</f>
         <v>5.3781512605042012</v>
       </c>
-      <c r="F14" s="1">
-        <f t="shared" ref="F14:F19" si="3">SUM(B14*B$12,C14*C$12,D14*D$12,E14*E$12)</f>
-        <v>5.7125782369933304</v>
-      </c>
-      <c r="G14" t="s">
+      <c r="G14" s="1">
+        <f t="shared" ref="G14:G19" si="3">SUM(B14*B$12,D14*D$12,E14*E$12,F14*F$12,C14*C$12)</f>
+        <v>6.806459565402962</v>
+      </c>
+      <c r="H14" s="5" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>45</v>
       </c>
@@ -1627,26 +1673,29 @@
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="C15">
+      <c r="C15" s="1">
+        <v>10</v>
+      </c>
+      <c r="D15">
         <v>5</v>
       </c>
-      <c r="D15" s="1">
+      <c r="E15" s="1">
         <f t="shared" si="1"/>
         <v>2.0517074683544303</v>
       </c>
-      <c r="E15" s="1">
+      <c r="F15" s="1">
         <f t="shared" si="2"/>
         <v>2.6666666666666665</v>
       </c>
-      <c r="F15" s="1">
+      <c r="G15" s="1">
         <f t="shared" si="3"/>
-        <v>4.4155122405063292</v>
-      </c>
-      <c r="G15" t="s">
+        <v>6.4436748270042195</v>
+      </c>
+      <c r="H15" s="5" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>49</v>
       </c>
@@ -1654,26 +1703,29 @@
         <f t="shared" si="0"/>
         <v>2.0977777777777775</v>
       </c>
-      <c r="C16">
+      <c r="C16" s="1">
+        <v>10</v>
+      </c>
+      <c r="D16">
         <v>5</v>
       </c>
-      <c r="D16" s="1">
+      <c r="E16" s="1">
         <f t="shared" si="1"/>
         <v>10</v>
       </c>
-      <c r="E16" s="1">
+      <c r="F16" s="1">
         <f t="shared" si="2"/>
         <v>8.0200501253132828</v>
       </c>
-      <c r="F16" s="1">
+      <c r="G16" s="1">
         <f t="shared" si="3"/>
-        <v>6.8255705931495401</v>
-      </c>
-      <c r="G16" t="s">
+        <v>7.5235655806182118</v>
+      </c>
+      <c r="H16" s="5" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>50</v>
       </c>
@@ -1681,26 +1733,29 @@
         <f t="shared" si="0"/>
         <v>2.0977777777777775</v>
       </c>
-      <c r="C17">
-        <v>10</v>
-      </c>
-      <c r="D17" s="1">
+      <c r="C17" s="1">
+        <v>5</v>
+      </c>
+      <c r="D17">
+        <v>10</v>
+      </c>
+      <c r="E17" s="1">
         <f t="shared" si="1"/>
         <v>10</v>
       </c>
-      <c r="E17" s="1">
+      <c r="F17" s="1">
         <f t="shared" si="2"/>
         <v>6.4128256513026045</v>
       </c>
-      <c r="F17" s="1">
+      <c r="G17" s="1">
         <f t="shared" si="3"/>
-        <v>7.3434032509463378</v>
-      </c>
-      <c r="G17" s="5" t="s">
+        <v>6.2021206858160767</v>
+      </c>
+      <c r="H17" s="5" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>53</v>
       </c>
@@ -1708,26 +1763,29 @@
         <f t="shared" si="0"/>
         <v>2.3111111111111113</v>
       </c>
-      <c r="C18">
+      <c r="C18" s="1">
+        <v>10</v>
+      </c>
+      <c r="D18">
         <v>5</v>
       </c>
-      <c r="D18" s="1">
+      <c r="E18" s="1">
         <f t="shared" si="1"/>
         <v>5.5556709905310342</v>
       </c>
-      <c r="E18" s="1">
+      <c r="F18" s="1">
         <f t="shared" si="2"/>
         <v>6.4646464646464654</v>
       </c>
-      <c r="F18" s="1">
+      <c r="G18" s="1">
         <f t="shared" si="3"/>
-        <v>5.0683174587754722</v>
-      </c>
-      <c r="G18" t="s">
+        <v>6.3662857132577226</v>
+      </c>
+      <c r="H18" s="5" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>56</v>
       </c>
@@ -1735,32 +1793,41 @@
         <f t="shared" si="0"/>
         <v>3.8559999999999999</v>
       </c>
-      <c r="C19">
+      <c r="C19" s="1">
+        <v>10</v>
+      </c>
+      <c r="D19">
         <v>5</v>
       </c>
-      <c r="D19" s="1">
+      <c r="E19" s="1">
         <f t="shared" si="1"/>
         <v>5.0353779930051124</v>
       </c>
-      <c r="E19" s="1">
+      <c r="F19" s="1">
         <f t="shared" si="2"/>
         <v>10</v>
       </c>
-      <c r="F19" s="1">
+      <c r="G19" s="1">
         <f t="shared" si="3"/>
-        <v>6.2818133979015336</v>
-      </c>
-      <c r="G19" t="s">
+        <v>7.2782755986010219</v>
+      </c>
+      <c r="H19" s="5" t="s">
         <v>55</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="F1:F2"/>
-    <mergeCell ref="F11:F12"/>
+    <mergeCell ref="G1:G2"/>
+    <mergeCell ref="G11:G12"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="G17" r:id="rId1"/>
+    <hyperlink ref="H17" r:id="rId1"/>
+    <hyperlink ref="H13" r:id="rId2"/>
+    <hyperlink ref="H14" r:id="rId3"/>
+    <hyperlink ref="H16" r:id="rId4"/>
+    <hyperlink ref="H15" r:id="rId5"/>
+    <hyperlink ref="H18" r:id="rId6" location="Dimensions"/>
+    <hyperlink ref="H19" r:id="rId7"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
worked on servos section
</commit_message>
<xml_diff>
--- a/Motor and Servo Decision Matrices.xlsx
+++ b/Motor and Servo Decision Matrices.xlsx
@@ -582,7 +582,7 @@
   <dimension ref="A1:J29"/>
   <sheetViews>
     <sheetView topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1341,7 +1341,7 @@
   <dimension ref="A1:H19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H19" sqref="H19"/>
+      <selection sqref="A1:F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>